<commit_message>
bot5 terminado al 100% version 1.0
</commit_message>
<xml_diff>
--- a/BASE DE DATOS DIST.xlsx
+++ b/BASE DE DATOS DIST.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Traslado de tesoreria B5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{BE8AD11F-7A6F-4F57-950D-0D437EC88447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3541E045-1859-4367-A69B-98CC1F0EB064}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{BE8AD11F-7A6F-4F57-950D-0D437EC88447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C22C57CF-B4CE-4707-8BB4-6BCE2B48D62A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82260D2F-9B51-457D-93F8-1C237327D8D4}"/>
+    <workbookView xWindow="-21720" yWindow="570" windowWidth="21840" windowHeight="13020" xr2:uid="{82260D2F-9B51-457D-93F8-1C237327D8D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -579,9 +579,6 @@
     <t xml:space="preserve">ISRAEL OCAMPO CAYOJA </t>
   </si>
   <si>
-    <t>FULVIA GUZMÁN OLIVARES</t>
-  </si>
-  <si>
     <t>VALERY DANIA TERCEROS RAMIREZ</t>
   </si>
   <si>
@@ -607,6 +604,9 @@
   </si>
   <si>
     <t xml:space="preserve">FABIOLA NAVA DURAN  </t>
+  </si>
+  <si>
+    <t>FULVIA GUZMAN OLIVARES</t>
   </si>
 </sst>
 </file>
@@ -839,10 +839,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1160,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB3360B-3B05-4F09-917C-967FB78A7C0E}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,7 +1256,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="25" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="11" t="s">
@@ -1273,7 +1273,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="11" t="s">
         <v>116</v>
       </c>
@@ -1286,7 +1286,7 @@
       <c r="E7" s="13"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="11"/>
       <c r="C8" s="13"/>
       <c r="D8" t="s">
@@ -1314,7 +1314,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="26" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="12"/>
@@ -1327,7 +1327,7 @@
       <c r="E10" s="12"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="12" t="s">
         <v>117</v>
       </c>
@@ -1342,7 +1342,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
       <c r="D12" t="s">
@@ -1351,7 +1351,7 @@
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="25" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="11" t="s">
@@ -1368,7 +1368,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="11" t="s">
         <v>121</v>
       </c>
@@ -1383,7 +1383,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="11" t="s">
@@ -1400,7 +1400,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="11" t="s">
         <v>123</v>
       </c>
@@ -1415,7 +1415,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="11" t="s">
         <v>123</v>
       </c>
@@ -1430,7 +1430,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="11" t="s">
         <v>123</v>
       </c>
@@ -1445,7 +1445,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="11" t="s">
         <v>123</v>
       </c>
@@ -1460,7 +1460,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="11" t="s">
         <v>123</v>
       </c>
@@ -1475,7 +1475,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="11" t="s">
@@ -1492,7 +1492,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="11" t="s">
         <v>125</v>
       </c>
@@ -1654,7 +1654,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="25" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="11"/>
@@ -1669,7 +1669,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11" t="s">
         <v>34</v>
@@ -1682,7 +1682,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
+      <c r="A34" s="25"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11" t="s">
         <v>36</v>
@@ -1712,7 +1712,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="25" t="s">
         <v>38</v>
       </c>
       <c r="B36" s="11"/>
@@ -1727,7 +1727,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
+      <c r="A37" s="25"/>
       <c r="B37" s="11"/>
       <c r="C37" s="12" t="s">
         <v>42</v>
@@ -1740,20 +1740,20 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="26"/>
+      <c r="A38" s="25"/>
       <c r="B38" s="11"/>
       <c r="C38" s="12" t="s">
         <v>44</v>
       </c>
       <c r="D38" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="E38" s="11" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="26" t="s">
+      <c r="A39" s="25" t="s">
         <v>46</v>
       </c>
       <c r="B39" s="11"/>
@@ -1768,7 +1768,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="11"/>
       <c r="C40" s="20" t="s">
         <v>48</v>
@@ -1781,7 +1781,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="26" t="s">
+      <c r="A41" s="25" t="s">
         <v>49</v>
       </c>
       <c r="B41" s="11" t="s">
@@ -1798,7 +1798,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
+      <c r="A42" s="25"/>
       <c r="B42" s="11" t="s">
         <v>123</v>
       </c>
@@ -1813,7 +1813,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="26" t="s">
+      <c r="A43" s="25" t="s">
         <v>49</v>
       </c>
       <c r="B43" s="11"/>
@@ -1828,7 +1828,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
+      <c r="A44" s="25"/>
       <c r="B44" s="11"/>
       <c r="C44" s="20" t="s">
         <v>51</v>
@@ -1871,7 +1871,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="25" t="s">
+      <c r="A47" s="26" t="s">
         <v>58</v>
       </c>
       <c r="B47" s="12"/>
@@ -1886,7 +1886,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="25"/>
+      <c r="A48" s="26"/>
       <c r="B48" s="12"/>
       <c r="C48" s="11" t="s">
         <v>61</v>
@@ -1899,7 +1899,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="25" t="s">
+      <c r="A49" s="26" t="s">
         <v>63</v>
       </c>
       <c r="B49" s="12"/>
@@ -1914,7 +1914,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="25"/>
+      <c r="A50" s="26"/>
       <c r="B50" s="12"/>
       <c r="C50" s="11" t="s">
         <v>66</v>
@@ -1927,7 +1927,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="25"/>
+      <c r="A51" s="26"/>
       <c r="B51" s="12"/>
       <c r="C51" s="11" t="s">
         <v>68</v>
@@ -1940,7 +1940,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="25" t="s">
+      <c r="A52" s="26" t="s">
         <v>70</v>
       </c>
       <c r="B52" s="12"/>
@@ -1955,7 +1955,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="25"/>
+      <c r="A53" s="26"/>
       <c r="B53" s="12"/>
       <c r="C53" s="11" t="s">
         <v>73</v>
@@ -1968,7 +1968,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="25" t="s">
+      <c r="A54" s="26" t="s">
         <v>75</v>
       </c>
       <c r="B54" s="12"/>
@@ -1983,7 +1983,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="25"/>
+      <c r="A55" s="26"/>
       <c r="B55" s="12"/>
       <c r="C55" s="11" t="s">
         <v>78</v>
@@ -1996,7 +1996,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="25" t="s">
+      <c r="A56" s="26" t="s">
         <v>80</v>
       </c>
       <c r="B56" s="12"/>
@@ -2011,7 +2011,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="25"/>
+      <c r="A57" s="26"/>
       <c r="B57" s="12"/>
       <c r="C57" s="11" t="s">
         <v>83</v>
@@ -2024,7 +2024,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="25"/>
+      <c r="A58" s="26"/>
       <c r="B58" s="12"/>
       <c r="C58" s="11" t="s">
         <v>85</v>
@@ -2045,7 +2045,7 @@
         <v>88</v>
       </c>
       <c r="D59" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E59" s="14" t="s">
         <v>89</v>
@@ -2060,7 +2060,7 @@
         <v>90</v>
       </c>
       <c r="D60" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E60" s="19" t="s">
         <v>91</v>
@@ -2075,12 +2075,12 @@
         <v>131</v>
       </c>
       <c r="D61" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E61" s="24"/>
     </row>
     <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="25" t="s">
+      <c r="A62" s="26" t="s">
         <v>101</v>
       </c>
       <c r="B62" s="12" t="s">
@@ -2090,14 +2090,14 @@
         <v>132</v>
       </c>
       <c r="D62" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E62" s="12" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="25"/>
+      <c r="A63" s="26"/>
       <c r="B63" s="12" t="s">
         <v>126</v>
       </c>
@@ -2105,12 +2105,12 @@
         <v>129</v>
       </c>
       <c r="D63" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E63" s="12"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="25"/>
+      <c r="A64" s="26"/>
       <c r="B64" s="12" t="s">
         <v>116</v>
       </c>
@@ -2118,12 +2118,12 @@
         <v>130</v>
       </c>
       <c r="D64" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E64" s="12"/>
     </row>
     <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="25" t="s">
+      <c r="A65" s="26" t="s">
         <v>102</v>
       </c>
       <c r="B65" s="12" t="s">
@@ -2133,14 +2133,14 @@
         <v>160</v>
       </c>
       <c r="D65" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E65" s="12" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="25" t="s">
+      <c r="A66" s="26" t="s">
         <v>103</v>
       </c>
       <c r="B66" s="12" t="s">
@@ -2150,14 +2150,14 @@
         <v>133</v>
       </c>
       <c r="D66" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E66" s="11" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A67" s="25" t="s">
+      <c r="A67" s="26" t="s">
         <v>103</v>
       </c>
       <c r="B67" s="12" t="s">
@@ -2167,7 +2167,7 @@
         <v>135</v>
       </c>
       <c r="D67" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E67" s="11" t="s">
         <v>105</v>
@@ -2175,11 +2175,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="A21:A22"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="A49:A51"/>
     <mergeCell ref="A32:A34"/>
@@ -2192,6 +2187,11 @@
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A41:A42"/>
     <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="A21:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
bot5 finalizado version 1.01
</commit_message>
<xml_diff>
--- a/BASE DE DATOS DIST.xlsx
+++ b/BASE DE DATOS DIST.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{BE8AD11F-7A6F-4F57-950D-0D437EC88447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C22C57CF-B4CE-4707-8BB4-6BCE2B48D62A}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{BE8AD11F-7A6F-4F57-950D-0D437EC88447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E737A28-B0DE-48B1-BB3D-662A6AD982D9}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="570" windowWidth="21840" windowHeight="13020" xr2:uid="{82260D2F-9B51-457D-93F8-1C237327D8D4}"/>
+    <workbookView xWindow="4830" yWindow="5520" windowWidth="17025" windowHeight="7470" xr2:uid="{82260D2F-9B51-457D-93F8-1C237327D8D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$E$67</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -859,6 +862,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1160,7 +1167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB3360B-3B05-4F09-917C-967FB78A7C0E}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -2174,6 +2181,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E67" xr:uid="{FCB3360B-3B05-4F09-917C-967FB78A7C0E}"/>
   <mergeCells count="17">
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="A49:A51"/>

</xml_diff>

<commit_message>
intermedio de bot5GUI -v 1.0
</commit_message>
<xml_diff>
--- a/BASE DE DATOS DIST.xlsx
+++ b/BASE DE DATOS DIST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{BE8AD11F-7A6F-4F57-950D-0D437EC88447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E737A28-B0DE-48B1-BB3D-662A6AD982D9}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{BE8AD11F-7A6F-4F57-950D-0D437EC88447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95866986-EF0B-46FF-BEB8-176CDCA4937B}"/>
   <bookViews>
-    <workbookView xWindow="4830" yWindow="5520" windowWidth="17025" windowHeight="7470" xr2:uid="{82260D2F-9B51-457D-93F8-1C237327D8D4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82260D2F-9B51-457D-93F8-1C237327D8D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1167,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB3360B-3B05-4F09-917C-967FB78A7C0E}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Bot5GUI --v1.01 - falta probar directo y varias asignaciones a la vez
</commit_message>
<xml_diff>
--- a/BASE DE DATOS DIST.xlsx
+++ b/BASE DE DATOS DIST.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{BE8AD11F-7A6F-4F57-950D-0D437EC88447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95866986-EF0B-46FF-BEB8-176CDCA4937B}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{BE8AD11F-7A6F-4F57-950D-0D437EC88447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAD464D8-9A1A-4FA1-8843-E5A0D7375932}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82260D2F-9B51-457D-93F8-1C237327D8D4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{82260D2F-9B51-457D-93F8-1C237327D8D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -862,10 +862,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1157,7 +1153,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1167,8 +1163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB3360B-3B05-4F09-917C-967FB78A7C0E}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Bot5GUI --v 1.01 SOLO AGENCIAS probadas
</commit_message>
<xml_diff>
--- a/BASE DE DATOS DIST.xlsx
+++ b/BASE DE DATOS DIST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{BE8AD11F-7A6F-4F57-950D-0D437EC88447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAD464D8-9A1A-4FA1-8843-E5A0D7375932}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{BE8AD11F-7A6F-4F57-950D-0D437EC88447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E957072A-9D36-451F-9983-2204B4CBA09A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{82260D2F-9B51-457D-93F8-1C237327D8D4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="192">
   <si>
     <t>Agencia / Distribuidora</t>
   </si>
@@ -585,9 +585,6 @@
     <t>VALERY DANIA TERCEROS RAMIREZ</t>
   </si>
   <si>
-    <t>ERICK EDUARDO IBAÑEZ ZAPATA</t>
-  </si>
-  <si>
     <t xml:space="preserve">ANA MARIA VEGA PEREYRA </t>
   </si>
   <si>
@@ -597,9 +594,6 @@
     <t xml:space="preserve"> MARCIAL ZELAYA VARGAS</t>
   </si>
   <si>
-    <t>JUAN XAVIER AVENDAÑO DURAN</t>
-  </si>
-  <si>
     <t>CHRISTIAN FERMANDO MONTERO</t>
   </si>
   <si>
@@ -610,6 +604,15 @@
   </si>
   <si>
     <t>FULVIA GUZMAN OLIVARES</t>
+  </si>
+  <si>
+    <t>FERNANDEZ PAUNI DAVID</t>
+  </si>
+  <si>
+    <t>ERICK EDUARDO IBAEZ ZAPATA</t>
+  </si>
+  <si>
+    <t>JUAN XAVIER AVENDAO DURAN</t>
   </si>
 </sst>
 </file>
@@ -842,10 +845,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -862,6 +865,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1163,8 +1170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB3360B-3B05-4F09-917C-967FB78A7C0E}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1259,7 +1266,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="26" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="11" t="s">
@@ -1276,7 +1283,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="11" t="s">
         <v>116</v>
       </c>
@@ -1289,7 +1296,7 @@
       <c r="E7" s="13"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="11"/>
       <c r="C8" s="13"/>
       <c r="D8" t="s">
@@ -1317,7 +1324,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="25" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="12"/>
@@ -1330,7 +1337,7 @@
       <c r="E10" s="12"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="12" t="s">
         <v>117</v>
       </c>
@@ -1345,7 +1352,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
       <c r="D12" t="s">
@@ -1354,7 +1361,7 @@
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="26" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="11" t="s">
@@ -1371,7 +1378,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="11" t="s">
         <v>121</v>
       </c>
@@ -1386,7 +1393,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="11" t="s">
@@ -1403,7 +1410,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="11" t="s">
         <v>123</v>
       </c>
@@ -1418,7 +1425,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="11" t="s">
         <v>123</v>
       </c>
@@ -1433,7 +1440,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="11" t="s">
         <v>123</v>
       </c>
@@ -1448,7 +1455,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="11" t="s">
         <v>123</v>
       </c>
@@ -1463,7 +1470,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="11" t="s">
         <v>123</v>
       </c>
@@ -1478,7 +1485,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="11" t="s">
@@ -1495,7 +1502,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="11" t="s">
         <v>125</v>
       </c>
@@ -1657,7 +1664,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="26" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="11"/>
@@ -1672,7 +1679,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11" t="s">
         <v>34</v>
@@ -1685,7 +1692,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
+      <c r="A34" s="26"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11" t="s">
         <v>36</v>
@@ -1715,7 +1722,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="26" t="s">
         <v>38</v>
       </c>
       <c r="B36" s="11"/>
@@ -1730,7 +1737,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="11"/>
       <c r="C37" s="12" t="s">
         <v>42</v>
@@ -1743,20 +1750,20 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
+      <c r="A38" s="26"/>
       <c r="B38" s="11"/>
       <c r="C38" s="12" t="s">
         <v>44</v>
       </c>
       <c r="D38" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E38" s="11" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="25" t="s">
+      <c r="A39" s="26" t="s">
         <v>46</v>
       </c>
       <c r="B39" s="11"/>
@@ -1771,7 +1778,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
+      <c r="A40" s="26"/>
       <c r="B40" s="11"/>
       <c r="C40" s="20" t="s">
         <v>48</v>
@@ -1784,7 +1791,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="25" t="s">
+      <c r="A41" s="26" t="s">
         <v>49</v>
       </c>
       <c r="B41" s="11" t="s">
@@ -1801,7 +1808,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="25"/>
+      <c r="A42" s="26"/>
       <c r="B42" s="11" t="s">
         <v>123</v>
       </c>
@@ -1816,7 +1823,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="26" t="s">
         <v>49</v>
       </c>
       <c r="B43" s="11"/>
@@ -1831,7 +1838,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
+      <c r="A44" s="26"/>
       <c r="B44" s="11"/>
       <c r="C44" s="20" t="s">
         <v>51</v>
@@ -1874,7 +1881,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="26" t="s">
+      <c r="A47" s="25" t="s">
         <v>58</v>
       </c>
       <c r="B47" s="12"/>
@@ -1889,7 +1896,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="26"/>
+      <c r="A48" s="25"/>
       <c r="B48" s="12"/>
       <c r="C48" s="11" t="s">
         <v>61</v>
@@ -1902,7 +1909,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="26" t="s">
+      <c r="A49" s="25" t="s">
         <v>63</v>
       </c>
       <c r="B49" s="12"/>
@@ -1917,7 +1924,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="26"/>
+      <c r="A50" s="25"/>
       <c r="B50" s="12"/>
       <c r="C50" s="11" t="s">
         <v>66</v>
@@ -1930,7 +1937,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="26"/>
+      <c r="A51" s="25"/>
       <c r="B51" s="12"/>
       <c r="C51" s="11" t="s">
         <v>68</v>
@@ -1943,7 +1950,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="26" t="s">
+      <c r="A52" s="25" t="s">
         <v>70</v>
       </c>
       <c r="B52" s="12"/>
@@ -1958,7 +1965,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="26"/>
+      <c r="A53" s="25"/>
       <c r="B53" s="12"/>
       <c r="C53" s="11" t="s">
         <v>73</v>
@@ -1971,7 +1978,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="26" t="s">
+      <c r="A54" s="25" t="s">
         <v>75</v>
       </c>
       <c r="B54" s="12"/>
@@ -1986,7 +1993,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="26"/>
+      <c r="A55" s="25"/>
       <c r="B55" s="12"/>
       <c r="C55" s="11" t="s">
         <v>78</v>
@@ -1999,7 +2006,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="26" t="s">
+      <c r="A56" s="25" t="s">
         <v>80</v>
       </c>
       <c r="B56" s="12"/>
@@ -2014,7 +2021,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="26"/>
+      <c r="A57" s="25"/>
       <c r="B57" s="12"/>
       <c r="C57" s="11" t="s">
         <v>83</v>
@@ -2027,13 +2034,13 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="26"/>
+      <c r="A58" s="25"/>
       <c r="B58" s="12"/>
       <c r="C58" s="11" t="s">
         <v>85</v>
       </c>
       <c r="D58" t="s">
-        <v>85</v>
+        <v>189</v>
       </c>
       <c r="E58" s="11" t="s">
         <v>86</v>
@@ -2063,7 +2070,7 @@
         <v>90</v>
       </c>
       <c r="D60" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="E60" s="19" t="s">
         <v>91</v>
@@ -2078,12 +2085,12 @@
         <v>131</v>
       </c>
       <c r="D61" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E61" s="24"/>
     </row>
     <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="26" t="s">
+      <c r="A62" s="25" t="s">
         <v>101</v>
       </c>
       <c r="B62" s="12" t="s">
@@ -2093,14 +2100,14 @@
         <v>132</v>
       </c>
       <c r="D62" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E62" s="12" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="26"/>
+      <c r="A63" s="25"/>
       <c r="B63" s="12" t="s">
         <v>126</v>
       </c>
@@ -2108,12 +2115,12 @@
         <v>129</v>
       </c>
       <c r="D63" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E63" s="12"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="26"/>
+      <c r="A64" s="25"/>
       <c r="B64" s="12" t="s">
         <v>116</v>
       </c>
@@ -2121,12 +2128,12 @@
         <v>130</v>
       </c>
       <c r="D64" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="E64" s="12"/>
     </row>
     <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="26" t="s">
+      <c r="A65" s="25" t="s">
         <v>102</v>
       </c>
       <c r="B65" s="12" t="s">
@@ -2136,14 +2143,14 @@
         <v>160</v>
       </c>
       <c r="D65" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E65" s="12" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="26" t="s">
+      <c r="A66" s="25" t="s">
         <v>103</v>
       </c>
       <c r="B66" s="12" t="s">
@@ -2153,14 +2160,14 @@
         <v>133</v>
       </c>
       <c r="D66" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E66" s="11" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A67" s="26" t="s">
+      <c r="A67" s="25" t="s">
         <v>103</v>
       </c>
       <c r="B67" s="12" t="s">
@@ -2170,7 +2177,7 @@
         <v>135</v>
       </c>
       <c r="D67" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E67" s="11" t="s">
         <v>105</v>
@@ -2179,6 +2186,11 @@
   </sheetData>
   <autoFilter ref="A1:E67" xr:uid="{FCB3360B-3B05-4F09-917C-967FB78A7C0E}"/>
   <mergeCells count="17">
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="A21:A22"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="A49:A51"/>
     <mergeCell ref="A32:A34"/>
@@ -2191,11 +2203,6 @@
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A41:A42"/>
     <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="A21:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Bot5 GUI testeada 260123
</commit_message>
<xml_diff>
--- a/BASE DE DATOS DIST.xlsx
+++ b/BASE DE DATOS DIST.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Bot5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://industriasvenado-my.sharepoint.com/personal/felipevillarroel_grupovenado_com/Documents/Proyecto Automatización Procesos Contables y Tesoreria/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{BE8AD11F-7A6F-4F57-950D-0D437EC88447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E957072A-9D36-451F-9983-2204B4CBA09A}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{BE8AD11F-7A6F-4F57-950D-0D437EC88447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1BE3741-1EF2-4ACE-A509-EED402611CA4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{82260D2F-9B51-457D-93F8-1C237327D8D4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$E$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$E$69</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="194">
   <si>
     <t>Agencia / Distribuidora</t>
   </si>
@@ -555,9 +555,6 @@
     <t>WILDER DARCO REQUENA ANTEZANA</t>
   </si>
   <si>
-    <t>JOAQUÍN CAMPERO SALAZAR</t>
-  </si>
-  <si>
     <t>RONALD OSINAGA MENACHO</t>
   </si>
   <si>
@@ -613,6 +610,15 @@
   </si>
   <si>
     <t>JUAN XAVIER AVENDAO DURAN</t>
+  </si>
+  <si>
+    <t>JOAQUIN CAMPERO SALAZAR</t>
+  </si>
+  <si>
+    <t>RODRIGUEZ CAIHUARA ARMIN</t>
+  </si>
+  <si>
+    <t>VICTOR MAURICIO MORALES</t>
   </si>
 </sst>
 </file>
@@ -865,10 +871,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1160,7 +1162,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1168,10 +1170,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB3360B-3B05-4F09-917C-967FB78A7C0E}">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1595,7 +1597,7 @@
         <v>154</v>
       </c>
       <c r="D27" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>26</v>
@@ -1612,7 +1614,7 @@
         <v>155</v>
       </c>
       <c r="D28" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>27</v>
@@ -1644,7 +1646,7 @@
         <v>156</v>
       </c>
       <c r="D30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E30" s="14"/>
     </row>
@@ -1672,7 +1674,7 @@
         <v>32</v>
       </c>
       <c r="D32" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>33</v>
@@ -1685,7 +1687,7 @@
         <v>34</v>
       </c>
       <c r="D33" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>35</v>
@@ -1698,7 +1700,7 @@
         <v>36</v>
       </c>
       <c r="D34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E34" s="11" t="s">
         <v>37</v>
@@ -1715,7 +1717,7 @@
         <v>157</v>
       </c>
       <c r="D35" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E35" s="11" t="s">
         <v>39</v>
@@ -1730,7 +1732,7 @@
         <v>40</v>
       </c>
       <c r="D36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>41</v>
@@ -1743,7 +1745,7 @@
         <v>42</v>
       </c>
       <c r="D37" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E37" s="11" t="s">
         <v>43</v>
@@ -1756,7 +1758,7 @@
         <v>44</v>
       </c>
       <c r="D38" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E38" s="11" t="s">
         <v>45</v>
@@ -2040,7 +2042,7 @@
         <v>85</v>
       </c>
       <c r="D58" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E58" s="11" t="s">
         <v>86</v>
@@ -2055,7 +2057,7 @@
         <v>88</v>
       </c>
       <c r="D59" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E59" s="14" t="s">
         <v>89</v>
@@ -2070,7 +2072,7 @@
         <v>90</v>
       </c>
       <c r="D60" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E60" s="19" t="s">
         <v>91</v>
@@ -2085,7 +2087,7 @@
         <v>131</v>
       </c>
       <c r="D61" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E61" s="24"/>
     </row>
@@ -2100,7 +2102,7 @@
         <v>132</v>
       </c>
       <c r="D62" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E62" s="12" t="s">
         <v>106</v>
@@ -2115,7 +2117,7 @@
         <v>129</v>
       </c>
       <c r="D63" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E63" s="12"/>
     </row>
@@ -2128,7 +2130,7 @@
         <v>130</v>
       </c>
       <c r="D64" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E64" s="12"/>
     </row>
@@ -2143,7 +2145,7 @@
         <v>160</v>
       </c>
       <c r="D65" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E65" s="12" t="s">
         <v>107</v>
@@ -2160,7 +2162,7 @@
         <v>133</v>
       </c>
       <c r="D66" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E66" s="11" t="s">
         <v>104</v>
@@ -2177,14 +2179,24 @@
         <v>135</v>
       </c>
       <c r="D67" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E67" s="11" t="s">
         <v>105</v>
       </c>
     </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>193</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E67" xr:uid="{FCB3360B-3B05-4F09-917C-967FB78A7C0E}"/>
+  <autoFilter ref="A1:E69" xr:uid="{FCB3360B-3B05-4F09-917C-967FB78A7C0E}"/>
   <mergeCells count="17">
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A10:A12"/>

</xml_diff>

<commit_message>
Bot5 GUI --v 1.00 betas finales
</commit_message>
<xml_diff>
--- a/BASE DE DATOS DIST.xlsx
+++ b/BASE DE DATOS DIST.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://industriasvenado-my.sharepoint.com/personal/felipevillarroel_grupovenado_com/Documents/Proyecto Automatización Procesos Contables y Tesoreria/Bot5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{BE8AD11F-7A6F-4F57-950D-0D437EC88447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1BE3741-1EF2-4ACE-A509-EED402611CA4}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{BE8AD11F-7A6F-4F57-950D-0D437EC88447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7629F54-BACB-413B-8E57-83F833C760CD}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{82260D2F-9B51-457D-93F8-1C237327D8D4}"/>
   </bookViews>
@@ -851,10 +851,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1162,7 +1162,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1173,7 +1173,7 @@
   <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,7 +1268,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="25" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="11" t="s">
@@ -1285,7 +1285,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="11" t="s">
         <v>116</v>
       </c>
@@ -1298,7 +1298,7 @@
       <c r="E7" s="13"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="11"/>
       <c r="C8" s="13"/>
       <c r="D8" t="s">
@@ -1326,7 +1326,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="26" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="12"/>
@@ -1339,7 +1339,7 @@
       <c r="E10" s="12"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="12" t="s">
         <v>117</v>
       </c>
@@ -1354,7 +1354,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
       <c r="D12" t="s">
@@ -1363,7 +1363,7 @@
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="25" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="11" t="s">
@@ -1380,7 +1380,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="11" t="s">
         <v>121</v>
       </c>
@@ -1395,7 +1395,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="11" t="s">
@@ -1412,7 +1412,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="11" t="s">
         <v>123</v>
       </c>
@@ -1427,7 +1427,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="11" t="s">
         <v>123</v>
       </c>
@@ -1442,7 +1442,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="11" t="s">
         <v>123</v>
       </c>
@@ -1457,7 +1457,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="11" t="s">
         <v>123</v>
       </c>
@@ -1472,7 +1472,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="11" t="s">
         <v>123</v>
       </c>
@@ -1487,7 +1487,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="11" t="s">
@@ -1504,7 +1504,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="11" t="s">
         <v>125</v>
       </c>
@@ -1666,7 +1666,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="25" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="11"/>
@@ -1681,7 +1681,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11" t="s">
         <v>34</v>
@@ -1694,7 +1694,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
+      <c r="A34" s="25"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11" t="s">
         <v>36</v>
@@ -1724,7 +1724,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="25" t="s">
         <v>38</v>
       </c>
       <c r="B36" s="11"/>
@@ -1739,7 +1739,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
+      <c r="A37" s="25"/>
       <c r="B37" s="11"/>
       <c r="C37" s="12" t="s">
         <v>42</v>
@@ -1752,7 +1752,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="26"/>
+      <c r="A38" s="25"/>
       <c r="B38" s="11"/>
       <c r="C38" s="12" t="s">
         <v>44</v>
@@ -1765,7 +1765,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="26" t="s">
+      <c r="A39" s="25" t="s">
         <v>46</v>
       </c>
       <c r="B39" s="11"/>
@@ -1780,7 +1780,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="11"/>
       <c r="C40" s="20" t="s">
         <v>48</v>
@@ -1793,7 +1793,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="26" t="s">
+      <c r="A41" s="25" t="s">
         <v>49</v>
       </c>
       <c r="B41" s="11" t="s">
@@ -1810,7 +1810,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
+      <c r="A42" s="25"/>
       <c r="B42" s="11" t="s">
         <v>123</v>
       </c>
@@ -1825,7 +1825,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="26" t="s">
+      <c r="A43" s="25" t="s">
         <v>49</v>
       </c>
       <c r="B43" s="11"/>
@@ -1840,7 +1840,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
+      <c r="A44" s="25"/>
       <c r="B44" s="11"/>
       <c r="C44" s="20" t="s">
         <v>51</v>
@@ -1883,7 +1883,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="25" t="s">
+      <c r="A47" s="26" t="s">
         <v>58</v>
       </c>
       <c r="B47" s="12"/>
@@ -1898,7 +1898,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="25"/>
+      <c r="A48" s="26"/>
       <c r="B48" s="12"/>
       <c r="C48" s="11" t="s">
         <v>61</v>
@@ -1911,7 +1911,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="25" t="s">
+      <c r="A49" s="26" t="s">
         <v>63</v>
       </c>
       <c r="B49" s="12"/>
@@ -1926,7 +1926,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="25"/>
+      <c r="A50" s="26"/>
       <c r="B50" s="12"/>
       <c r="C50" s="11" t="s">
         <v>66</v>
@@ -1939,7 +1939,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="25"/>
+      <c r="A51" s="26"/>
       <c r="B51" s="12"/>
       <c r="C51" s="11" t="s">
         <v>68</v>
@@ -1952,7 +1952,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="25" t="s">
+      <c r="A52" s="26" t="s">
         <v>70</v>
       </c>
       <c r="B52" s="12"/>
@@ -1967,7 +1967,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="25"/>
+      <c r="A53" s="26"/>
       <c r="B53" s="12"/>
       <c r="C53" s="11" t="s">
         <v>73</v>
@@ -1980,7 +1980,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="25" t="s">
+      <c r="A54" s="26" t="s">
         <v>75</v>
       </c>
       <c r="B54" s="12"/>
@@ -1995,7 +1995,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="25"/>
+      <c r="A55" s="26"/>
       <c r="B55" s="12"/>
       <c r="C55" s="11" t="s">
         <v>78</v>
@@ -2008,7 +2008,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="25" t="s">
+      <c r="A56" s="26" t="s">
         <v>80</v>
       </c>
       <c r="B56" s="12"/>
@@ -2023,7 +2023,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="25"/>
+      <c r="A57" s="26"/>
       <c r="B57" s="12"/>
       <c r="C57" s="11" t="s">
         <v>83</v>
@@ -2036,7 +2036,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="25"/>
+      <c r="A58" s="26"/>
       <c r="B58" s="12"/>
       <c r="C58" s="11" t="s">
         <v>85</v>
@@ -2092,7 +2092,7 @@
       <c r="E61" s="24"/>
     </row>
     <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="25" t="s">
+      <c r="A62" s="26" t="s">
         <v>101</v>
       </c>
       <c r="B62" s="12" t="s">
@@ -2109,7 +2109,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="25"/>
+      <c r="A63" s="26"/>
       <c r="B63" s="12" t="s">
         <v>126</v>
       </c>
@@ -2122,7 +2122,7 @@
       <c r="E63" s="12"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="25"/>
+      <c r="A64" s="26"/>
       <c r="B64" s="12" t="s">
         <v>116</v>
       </c>
@@ -2135,7 +2135,7 @@
       <c r="E64" s="12"/>
     </row>
     <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="25" t="s">
+      <c r="A65" s="26" t="s">
         <v>102</v>
       </c>
       <c r="B65" s="12" t="s">
@@ -2152,7 +2152,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="25" t="s">
+      <c r="A66" s="26" t="s">
         <v>103</v>
       </c>
       <c r="B66" s="12" t="s">
@@ -2169,7 +2169,7 @@
       </c>
     </row>
     <row r="67" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A67" s="25" t="s">
+      <c r="A67" s="26" t="s">
         <v>103</v>
       </c>
       <c r="B67" s="12" t="s">
@@ -2198,11 +2198,6 @@
   </sheetData>
   <autoFilter ref="A1:E69" xr:uid="{FCB3360B-3B05-4F09-917C-967FB78A7C0E}"/>
   <mergeCells count="17">
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="A21:A22"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="A49:A51"/>
     <mergeCell ref="A32:A34"/>
@@ -2215,6 +2210,11 @@
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A41:A42"/>
     <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="A21:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Bot5 GUI - prod1
</commit_message>
<xml_diff>
--- a/BASE DE DATOS DIST.xlsx
+++ b/BASE DE DATOS DIST.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Users\Siticom\Documents\Cris\Bot5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://industriasvenado-my.sharepoint.com/personal/felipevillarroel_grupovenado_com/Documents/Proyecto Automatización Procesos Contables y Tesoreria/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D36A9E-566B-49F5-930F-E54530F762C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{91D36A9E-566B-49F5-930F-E54530F762C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA27DCF6-AC1E-4F23-BFB4-F8EF64C1B899}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{82260D2F-9B51-457D-93F8-1C237327D8D4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{82260D2F-9B51-457D-93F8-1C237327D8D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="195">
   <si>
     <t>Agencia / Distribuidora</t>
   </si>
@@ -619,6 +619,9 @@
   </si>
   <si>
     <t>VICTOR MAURICIO MORALES</t>
+  </si>
+  <si>
+    <t>MICHEL JOSEP LOPEZ CASTELLON</t>
   </si>
 </sst>
 </file>
@@ -851,10 +854,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1170,10 +1173,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB3360B-3B05-4F09-917C-967FB78A7C0E}">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,7 +1271,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="25" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="11" t="s">
@@ -1285,7 +1288,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="11" t="s">
         <v>116</v>
       </c>
@@ -1298,7 +1301,7 @@
       <c r="E7" s="13"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="11"/>
       <c r="C8" s="13"/>
       <c r="D8" t="s">
@@ -1326,7 +1329,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="26" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="12"/>
@@ -1339,7 +1342,7 @@
       <c r="E10" s="12"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="12" t="s">
         <v>117</v>
       </c>
@@ -1354,7 +1357,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
       <c r="D12" t="s">
@@ -1363,7 +1366,7 @@
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="25" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="11" t="s">
@@ -1380,7 +1383,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="11" t="s">
         <v>121</v>
       </c>
@@ -1395,7 +1398,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="11" t="s">
@@ -1412,7 +1415,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="11" t="s">
         <v>123</v>
       </c>
@@ -1427,7 +1430,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="11" t="s">
         <v>123</v>
       </c>
@@ -1442,7 +1445,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="11" t="s">
         <v>123</v>
       </c>
@@ -1457,7 +1460,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="11" t="s">
         <v>123</v>
       </c>
@@ -1472,7 +1475,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="11" t="s">
         <v>123</v>
       </c>
@@ -1487,7 +1490,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="11" t="s">
@@ -1504,7 +1507,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="11" t="s">
         <v>125</v>
       </c>
@@ -1666,7 +1669,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="25" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="11"/>
@@ -1681,7 +1684,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11" t="s">
         <v>34</v>
@@ -1694,7 +1697,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
+      <c r="A34" s="25"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11" t="s">
         <v>36</v>
@@ -1724,7 +1727,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="25" t="s">
         <v>38</v>
       </c>
       <c r="B36" s="11"/>
@@ -1739,7 +1742,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
+      <c r="A37" s="25"/>
       <c r="B37" s="11"/>
       <c r="C37" s="12" t="s">
         <v>42</v>
@@ -1752,7 +1755,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="26"/>
+      <c r="A38" s="25"/>
       <c r="B38" s="11"/>
       <c r="C38" s="12" t="s">
         <v>44</v>
@@ -1765,7 +1768,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="26" t="s">
+      <c r="A39" s="25" t="s">
         <v>46</v>
       </c>
       <c r="B39" s="11"/>
@@ -1780,7 +1783,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="11"/>
       <c r="C40" s="20" t="s">
         <v>48</v>
@@ -1793,7 +1796,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="26" t="s">
+      <c r="A41" s="25" t="s">
         <v>49</v>
       </c>
       <c r="B41" s="11" t="s">
@@ -1810,7 +1813,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
+      <c r="A42" s="25"/>
       <c r="B42" s="11" t="s">
         <v>123</v>
       </c>
@@ -1825,7 +1828,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="26" t="s">
+      <c r="A43" s="25" t="s">
         <v>49</v>
       </c>
       <c r="B43" s="11"/>
@@ -1840,7 +1843,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
+      <c r="A44" s="25"/>
       <c r="B44" s="11"/>
       <c r="C44" s="20" t="s">
         <v>51</v>
@@ -1883,7 +1886,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="25" t="s">
+      <c r="A47" s="26" t="s">
         <v>58</v>
       </c>
       <c r="B47" s="12"/>
@@ -1898,7 +1901,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="25"/>
+      <c r="A48" s="26"/>
       <c r="B48" s="12"/>
       <c r="C48" s="11" t="s">
         <v>61</v>
@@ -1911,7 +1914,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="25" t="s">
+      <c r="A49" s="26" t="s">
         <v>63</v>
       </c>
       <c r="B49" s="12"/>
@@ -1926,7 +1929,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="25"/>
+      <c r="A50" s="26"/>
       <c r="B50" s="12"/>
       <c r="C50" s="11" t="s">
         <v>66</v>
@@ -1939,7 +1942,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="25"/>
+      <c r="A51" s="26"/>
       <c r="B51" s="12"/>
       <c r="C51" s="11" t="s">
         <v>68</v>
@@ -1952,7 +1955,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="25" t="s">
+      <c r="A52" s="26" t="s">
         <v>70</v>
       </c>
       <c r="B52" s="12"/>
@@ -1967,7 +1970,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="25"/>
+      <c r="A53" s="26"/>
       <c r="B53" s="12"/>
       <c r="C53" s="11" t="s">
         <v>73</v>
@@ -1980,7 +1983,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="25" t="s">
+      <c r="A54" s="26" t="s">
         <v>75</v>
       </c>
       <c r="B54" s="12"/>
@@ -1995,7 +1998,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="25"/>
+      <c r="A55" s="26"/>
       <c r="B55" s="12"/>
       <c r="C55" s="11" t="s">
         <v>78</v>
@@ -2008,7 +2011,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="25" t="s">
+      <c r="A56" s="26" t="s">
         <v>80</v>
       </c>
       <c r="B56" s="12"/>
@@ -2023,7 +2026,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="25"/>
+      <c r="A57" s="26"/>
       <c r="B57" s="12"/>
       <c r="C57" s="11" t="s">
         <v>83</v>
@@ -2036,7 +2039,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="25"/>
+      <c r="A58" s="26"/>
       <c r="B58" s="12"/>
       <c r="C58" s="11" t="s">
         <v>85</v>
@@ -2092,7 +2095,7 @@
       <c r="E61" s="24"/>
     </row>
     <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="25" t="s">
+      <c r="A62" s="26" t="s">
         <v>101</v>
       </c>
       <c r="B62" s="12" t="s">
@@ -2109,7 +2112,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="25"/>
+      <c r="A63" s="26"/>
       <c r="B63" s="12" t="s">
         <v>126</v>
       </c>
@@ -2122,7 +2125,7 @@
       <c r="E63" s="12"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="25"/>
+      <c r="A64" s="26"/>
       <c r="B64" s="12" t="s">
         <v>116</v>
       </c>
@@ -2135,7 +2138,7 @@
       <c r="E64" s="12"/>
     </row>
     <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="25" t="s">
+      <c r="A65" s="26" t="s">
         <v>102</v>
       </c>
       <c r="B65" s="12" t="s">
@@ -2152,7 +2155,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="25" t="s">
+      <c r="A66" s="26" t="s">
         <v>103</v>
       </c>
       <c r="B66" s="12" t="s">
@@ -2169,7 +2172,7 @@
       </c>
     </row>
     <row r="67" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A67" s="25" t="s">
+      <c r="A67" s="26" t="s">
         <v>103</v>
       </c>
       <c r="B67" s="12" t="s">
@@ -2195,14 +2198,14 @@
         <v>193</v>
       </c>
     </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>194</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E69" xr:uid="{FCB3360B-3B05-4F09-917C-967FB78A7C0E}"/>
   <mergeCells count="17">
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="A21:A22"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="A49:A51"/>
     <mergeCell ref="A32:A34"/>
@@ -2215,6 +2218,11 @@
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A41:A42"/>
     <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="A21:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Bot5 GUI error inesperado en DISPAZ
</commit_message>
<xml_diff>
--- a/BASE DE DATOS DIST.xlsx
+++ b/BASE DE DATOS DIST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://industriasvenado-my.sharepoint.com/personal/felipevillarroel_grupovenado_com/Documents/Proyecto Automatización Procesos Contables y Tesoreria/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{91D36A9E-566B-49F5-930F-E54530F762C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B232A52E-D048-45D2-A20F-A4D3D83B85C7}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{91D36A9E-566B-49F5-930F-E54530F762C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F474A0CC-43D3-4257-A1D0-F098D517703E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{82260D2F-9B51-457D-93F8-1C237327D8D4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="198">
   <si>
     <t>Agencia / Distribuidora</t>
   </si>
@@ -625,6 +625,12 @@
   </si>
   <si>
     <t>JHONNNY PACAJES YUJRA</t>
+  </si>
+  <si>
+    <t>MARILYN LESLIE VIDAL RIOS</t>
+  </si>
+  <si>
+    <t>JHONNY IGNACIO FLORES LOPEZ</t>
   </si>
 </sst>
 </file>
@@ -1176,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB3360B-3B05-4F09-917C-967FB78A7C0E}">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1966,7 +1972,7 @@
         <v>71</v>
       </c>
       <c r="D52" t="s">
-        <v>71</v>
+        <v>197</v>
       </c>
       <c r="E52" s="11" t="s">
         <v>72</v>
@@ -2209,6 +2215,11 @@
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
         <v>195</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bot5 GUI implementacion corregida
</commit_message>
<xml_diff>
--- a/BASE DE DATOS DIST.xlsx
+++ b/BASE DE DATOS DIST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://industriasvenado-my.sharepoint.com/personal/felipevillarroel_grupovenado_com/Documents/Proyecto Automatización Procesos Contables y Tesoreria/Bot5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{91D36A9E-566B-49F5-930F-E54530F762C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F474A0CC-43D3-4257-A1D0-F098D517703E}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{91D36A9E-566B-49F5-930F-E54530F762C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B80466EF-4BF0-4C7B-8A80-EE3FCD244464}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{82260D2F-9B51-457D-93F8-1C237327D8D4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="199">
   <si>
     <t>Agencia / Distribuidora</t>
   </si>
@@ -591,9 +591,6 @@
     <t xml:space="preserve"> MARCIAL ZELAYA VARGAS</t>
   </si>
   <si>
-    <t>CHRISTIAN FERMANDO MONTERO</t>
-  </si>
-  <si>
     <t>MARTHA CARDOZO SAAVEDRA</t>
   </si>
   <si>
@@ -631,6 +628,12 @@
   </si>
   <si>
     <t>JHONNY IGNACIO FLORES LOPEZ</t>
+  </si>
+  <si>
+    <t>CHRISTIAN FERNANDO MONTERO ESPINOZA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OSCAR LOZYZA SALVATIERRA</t>
   </si>
 </sst>
 </file>
@@ -863,10 +866,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1182,10 +1185,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB3360B-3B05-4F09-917C-967FB78A7C0E}">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E80" sqref="E80"/>
+    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,7 +1283,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="25" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="11" t="s">
@@ -1297,7 +1300,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="11" t="s">
         <v>116</v>
       </c>
@@ -1310,7 +1313,7 @@
       <c r="E7" s="13"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="11"/>
       <c r="C8" s="13"/>
       <c r="D8" t="s">
@@ -1338,7 +1341,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="26" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="12"/>
@@ -1351,7 +1354,7 @@
       <c r="E10" s="12"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="12" t="s">
         <v>117</v>
       </c>
@@ -1366,7 +1369,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="12"/>
       <c r="C12" s="13"/>
       <c r="D12" t="s">
@@ -1375,7 +1378,7 @@
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="25" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="11" t="s">
@@ -1392,7 +1395,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="11" t="s">
         <v>121</v>
       </c>
@@ -1407,7 +1410,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="11" t="s">
@@ -1424,7 +1427,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="11" t="s">
         <v>123</v>
       </c>
@@ -1439,7 +1442,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="11" t="s">
         <v>123</v>
       </c>
@@ -1454,7 +1457,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="11" t="s">
         <v>123</v>
       </c>
@@ -1469,7 +1472,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="11" t="s">
         <v>123</v>
       </c>
@@ -1484,7 +1487,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="11" t="s">
         <v>123</v>
       </c>
@@ -1499,7 +1502,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="11" t="s">
@@ -1516,7 +1519,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="11" t="s">
         <v>125</v>
       </c>
@@ -1609,7 +1612,7 @@
         <v>154</v>
       </c>
       <c r="D27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>26</v>
@@ -1678,7 +1681,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="25" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="11"/>
@@ -1693,7 +1696,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11" t="s">
         <v>34</v>
@@ -1706,7 +1709,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
+      <c r="A34" s="25"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11" t="s">
         <v>36</v>
@@ -1736,7 +1739,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="25" t="s">
         <v>38</v>
       </c>
       <c r="B36" s="11"/>
@@ -1751,7 +1754,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
+      <c r="A37" s="25"/>
       <c r="B37" s="11"/>
       <c r="C37" s="12" t="s">
         <v>42</v>
@@ -1764,20 +1767,20 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="26"/>
+      <c r="A38" s="25"/>
       <c r="B38" s="11"/>
       <c r="C38" s="12" t="s">
         <v>44</v>
       </c>
       <c r="D38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E38" s="11" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="26" t="s">
+      <c r="A39" s="25" t="s">
         <v>46</v>
       </c>
       <c r="B39" s="11"/>
@@ -1792,7 +1795,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="11"/>
       <c r="C40" s="20" t="s">
         <v>48</v>
@@ -1805,7 +1808,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="26" t="s">
+      <c r="A41" s="25" t="s">
         <v>49</v>
       </c>
       <c r="B41" s="11" t="s">
@@ -1822,7 +1825,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
+      <c r="A42" s="25"/>
       <c r="B42" s="11" t="s">
         <v>123</v>
       </c>
@@ -1837,7 +1840,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="26" t="s">
+      <c r="A43" s="25" t="s">
         <v>49</v>
       </c>
       <c r="B43" s="11"/>
@@ -1852,7 +1855,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
+      <c r="A44" s="25"/>
       <c r="B44" s="11"/>
       <c r="C44" s="20" t="s">
         <v>51</v>
@@ -1895,7 +1898,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="25" t="s">
+      <c r="A47" s="26" t="s">
         <v>58</v>
       </c>
       <c r="B47" s="12"/>
@@ -1910,7 +1913,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="25"/>
+      <c r="A48" s="26"/>
       <c r="B48" s="12"/>
       <c r="C48" s="11" t="s">
         <v>61</v>
@@ -1923,7 +1926,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="25" t="s">
+      <c r="A49" s="26" t="s">
         <v>63</v>
       </c>
       <c r="B49" s="12"/>
@@ -1938,7 +1941,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="25"/>
+      <c r="A50" s="26"/>
       <c r="B50" s="12"/>
       <c r="C50" s="11" t="s">
         <v>66</v>
@@ -1951,7 +1954,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="25"/>
+      <c r="A51" s="26"/>
       <c r="B51" s="12"/>
       <c r="C51" s="11" t="s">
         <v>68</v>
@@ -1964,7 +1967,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="25" t="s">
+      <c r="A52" s="26" t="s">
         <v>70</v>
       </c>
       <c r="B52" s="12"/>
@@ -1972,14 +1975,14 @@
         <v>71</v>
       </c>
       <c r="D52" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E52" s="11" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="25"/>
+      <c r="A53" s="26"/>
       <c r="B53" s="12"/>
       <c r="C53" s="11" t="s">
         <v>73</v>
@@ -1992,7 +1995,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="25" t="s">
+      <c r="A54" s="26" t="s">
         <v>75</v>
       </c>
       <c r="B54" s="12"/>
@@ -2007,7 +2010,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="25"/>
+      <c r="A55" s="26"/>
       <c r="B55" s="12"/>
       <c r="C55" s="11" t="s">
         <v>78</v>
@@ -2020,7 +2023,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="25" t="s">
+      <c r="A56" s="26" t="s">
         <v>80</v>
       </c>
       <c r="B56" s="12"/>
@@ -2035,7 +2038,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="25"/>
+      <c r="A57" s="26"/>
       <c r="B57" s="12"/>
       <c r="C57" s="11" t="s">
         <v>83</v>
@@ -2048,13 +2051,13 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="25"/>
+      <c r="A58" s="26"/>
       <c r="B58" s="12"/>
       <c r="C58" s="11" t="s">
         <v>85</v>
       </c>
       <c r="D58" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E58" s="11" t="s">
         <v>86</v>
@@ -2084,7 +2087,7 @@
         <v>90</v>
       </c>
       <c r="D60" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E60" s="19" t="s">
         <v>91</v>
@@ -2104,7 +2107,7 @@
       <c r="E61" s="24"/>
     </row>
     <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="25" t="s">
+      <c r="A62" s="26" t="s">
         <v>101</v>
       </c>
       <c r="B62" s="12" t="s">
@@ -2121,7 +2124,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="25"/>
+      <c r="A63" s="26"/>
       <c r="B63" s="12" t="s">
         <v>126</v>
       </c>
@@ -2134,7 +2137,7 @@
       <c r="E63" s="12"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="25"/>
+      <c r="A64" s="26"/>
       <c r="B64" s="12" t="s">
         <v>116</v>
       </c>
@@ -2142,12 +2145,12 @@
         <v>130</v>
       </c>
       <c r="D64" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E64" s="12"/>
     </row>
     <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="25" t="s">
+      <c r="A65" s="26" t="s">
         <v>102</v>
       </c>
       <c r="B65" s="12" t="s">
@@ -2157,14 +2160,14 @@
         <v>160</v>
       </c>
       <c r="D65" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="E65" s="12" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="25" t="s">
+      <c r="A66" s="26" t="s">
         <v>103</v>
       </c>
       <c r="B66" s="12" t="s">
@@ -2174,14 +2177,14 @@
         <v>133</v>
       </c>
       <c r="D66" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E66" s="11" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A67" s="25" t="s">
+      <c r="A67" s="26" t="s">
         <v>103</v>
       </c>
       <c r="B67" s="12" t="s">
@@ -2191,7 +2194,7 @@
         <v>135</v>
       </c>
       <c r="D67" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E67" s="11" t="s">
         <v>105</v>
@@ -2199,37 +2202,37 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
-        <v>196</v>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E69" xr:uid="{FCB3360B-3B05-4F09-917C-967FB78A7C0E}"/>
   <mergeCells count="17">
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="A21:A22"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="A49:A51"/>
     <mergeCell ref="A32:A34"/>
@@ -2242,6 +2245,11 @@
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A41:A42"/>
     <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="A21:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>